<commit_message>
feat: added img url scanning feature in CSVtoPLANTS
</commit_message>
<xml_diff>
--- a/src/main/resources/testdata.xlsx
+++ b/src/main/resources/testdata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10323"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10411"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dharjianto/Documents/S21/275labs/project-team-11-1/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dharjianto/Documents/S21/275labs/project-team-11-1/src/main/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F88F71F5-FC5A-A745-A42D-4FC04C7802B4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05B115F7-CD89-4A41-B271-9DDD4C864073}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="15420" windowHeight="15960" xr2:uid="{B4604050-3C25-CB42-9683-8AF787393E61}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="14280" windowHeight="15920" xr2:uid="{B4604050-3C25-CB42-9683-8AF787393E61}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="37">
   <si>
     <t>genus</t>
   </si>
@@ -45,9 +45,6 @@
     <t>description</t>
   </si>
   <si>
-    <t>image</t>
-  </si>
-  <si>
     <t>leps</t>
   </si>
   <si>
@@ -69,9 +66,6 @@
     <t>h</t>
   </si>
   <si>
-    <t>justicia</t>
-  </si>
-  <si>
     <t>americana</t>
   </si>
   <si>
@@ -81,9 +75,6 @@
     <t>Justicia: named for James Justice; americana: of the Americas</t>
   </si>
   <si>
-    <t>ruellia</t>
-  </si>
-  <si>
     <t>caroliniensis</t>
   </si>
   <si>
@@ -93,52 +84,67 @@
     <t>spring-summer</t>
   </si>
   <si>
+    <t>americanus</t>
+  </si>
+  <si>
+    <t>american sweetflag</t>
+  </si>
+  <si>
+    <t>Acorus: plant with an aromatic rhizome; americanus: of the Americas</t>
+  </si>
+  <si>
+    <t>canadensis</t>
+  </si>
+  <si>
+    <t>elderberry</t>
+  </si>
+  <si>
+    <t>acerifolium</t>
+  </si>
+  <si>
+    <t>mapleleaf viburnum</t>
+  </si>
+  <si>
+    <t>Viburnum: Latin name for the wayfaring tree; acerifolium: leaves like a maple tree</t>
+  </si>
+  <si>
+    <t>Ruellia: named for Jean Ruel- 16th century French botanist; caroliniensis: of or from Carolina (U.S.)</t>
+  </si>
+  <si>
+    <t>Sambucus: named for the sambuca- a stringed instrument made from the elder wood; canadensis: of or from Canada and North America</t>
+  </si>
+  <si>
+    <t>Justicia</t>
+  </si>
+  <si>
+    <t>Ruellia</t>
+  </si>
+  <si>
+    <t>Acorus</t>
+  </si>
+  <si>
+    <t>Sambucus</t>
+  </si>
+  <si>
+    <t>Viburnum</t>
+  </si>
+  <si>
+    <t>image url</t>
+  </si>
+  <si>
     <t>https://www.wrc.udel.edu/wp-content/heritage/viewtn.php?photo_id=361</t>
   </si>
   <si>
-    <t>acorus</t>
-  </si>
-  <si>
-    <t>americanus</t>
-  </si>
-  <si>
-    <t>american sweetflag</t>
-  </si>
-  <si>
-    <t>Acorus: plant with an aromatic rhizome; americanus: of the Americas</t>
-  </si>
-  <si>
-    <t>sambucus</t>
-  </si>
-  <si>
-    <t>canadensis</t>
-  </si>
-  <si>
-    <t>elderberry</t>
-  </si>
-  <si>
-    <t>viburnum</t>
-  </si>
-  <si>
-    <t>acerifolium</t>
-  </si>
-  <si>
-    <t>https://www.wrc.udel.edu/wp-content/heritage/viewtn.php?photo_id=371</t>
-  </si>
-  <si>
-    <t>https://www.wrc.udel.edu/wp-content/heritage/viewtn.php?photo_id=2306</t>
-  </si>
-  <si>
-    <t>mapleleaf viburnum</t>
-  </si>
-  <si>
-    <t>Viburnum: Latin name for the wayfaring tree; acerifolium: leaves like a maple tree</t>
-  </si>
-  <si>
-    <t>Ruellia: named for Jean Ruel- 16th century French botanist; caroliniensis: of or from Carolina (U.S.)</t>
-  </si>
-  <si>
-    <t>Sambucus: named for the sambuca- a stringed instrument made from the elder wood; canadensis: of or from Canada and North America</t>
+    <t>https://www.wrc.udel.edu/wp-content/heritage/viewtn.php?photo_id=56</t>
+  </si>
+  <si>
+    <t>https://www.wrc.udel.edu/wp-content/heritage/viewtn.php?photo_id=1144</t>
+  </si>
+  <si>
+    <t>https://www.wrc.udel.edu/wp-content/heritage/viewtn.php?photo_id=1556</t>
+  </si>
+  <si>
+    <t>https://www.wrc.udel.edu/wp-content/heritage/viewtn.php?photo_id=1417</t>
   </si>
 </sst>
 </file>
@@ -536,7 +542,7 @@
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -555,137 +561,140 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D1" s="6" t="s">
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>5</v>
-      </c>
       <c r="H1" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="61" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
         <v>11</v>
       </c>
-      <c r="B2" t="s">
+      <c r="D2" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>14</v>
+      <c r="E2" t="s">
+        <v>34</v>
       </c>
       <c r="G2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="76" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="G3" t="s">
         <v>15</v>
       </c>
-      <c r="B3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="G3" t="s">
-        <v>18</v>
-      </c>
       <c r="H3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="61" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="B4" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C4" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>23</v>
+        <v>18</v>
+      </c>
+      <c r="E4" t="s">
+        <v>33</v>
       </c>
       <c r="G4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="106" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="B5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C5" t="s">
-        <v>26</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>34</v>
-      </c>
       <c r="E5" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="G5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B6" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="C6" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="E6" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="G6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="E3" r:id="rId1" xr:uid="{FF1E823A-42DA-C34B-B2AF-9F47510EBCBC}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>